<commit_message>
Added unfamiliar exercise phrases and the checkboxes show how many keywords are in the text
</commit_message>
<xml_diff>
--- a/Keyword Extraction/Results_Detailed Accuracy/detailedAccuracy_Video_2_nikeTrainerClub.txt.xlsx
+++ b/Keyword Extraction/Results_Detailed Accuracy/detailedAccuracy_Video_2_nikeTrainerClub.txt.xlsx
@@ -1972,7 +1972,7 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>99.99836683273315</v>
+        <v>99.99860525131226</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2027,7 +2027,7 @@
         <v>2</v>
       </c>
       <c r="D7">
-        <v>99.99179840087891</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -2038,7 +2038,7 @@
         <v>2</v>
       </c>
       <c r="D8">
-        <v>99.99998807907104</v>
+        <v>99.99995231628418</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -2060,7 +2060,7 @@
         <v>2</v>
       </c>
       <c r="D10">
-        <v>99.87642765045166</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -2082,7 +2082,7 @@
         <v>2</v>
       </c>
       <c r="D12">
-        <v>99.99973773956299</v>
+        <v>99.99986886978149</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -2093,7 +2093,7 @@
         <v>2</v>
       </c>
       <c r="D13">
-        <v>99.96359348297119</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -2101,10 +2101,10 @@
         <v>15</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D14">
-        <v>99.99032020568848</v>
+        <v>99.99997615814209</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -2115,7 +2115,7 @@
         <v>2</v>
       </c>
       <c r="D15">
-        <v>99.99678134918213</v>
+        <v>99.99997615814209</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -2137,7 +2137,7 @@
         <v>2</v>
       </c>
       <c r="D17">
-        <v>99.99998807907104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -2145,10 +2145,10 @@
         <v>19</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D18">
-        <v>99.59723353385925</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -2159,7 +2159,7 @@
         <v>2</v>
       </c>
       <c r="D19">
-        <v>99.97174143791199</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -2170,7 +2170,7 @@
         <v>2</v>
       </c>
       <c r="D20">
-        <v>100</v>
+        <v>99.99985694885254</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -2181,7 +2181,7 @@
         <v>2</v>
       </c>
       <c r="D21">
-        <v>99.99964237213135</v>
+        <v>99.9998927116394</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -2214,7 +2214,7 @@
         <v>2</v>
       </c>
       <c r="D24">
-        <v>99.99972581863403</v>
+        <v>99.99985694885254</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -2236,7 +2236,7 @@
         <v>2</v>
       </c>
       <c r="D26">
-        <v>99.99992847442627</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -2269,7 +2269,7 @@
         <v>2</v>
       </c>
       <c r="D29">
-        <v>99.99998807907104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -2280,7 +2280,7 @@
         <v>2</v>
       </c>
       <c r="D30">
-        <v>99.9995231628418</v>
+        <v>99.99997615814209</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -2313,7 +2313,7 @@
         <v>2</v>
       </c>
       <c r="D33">
-        <v>100</v>
+        <v>99.9998927116394</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -2335,7 +2335,7 @@
         <v>1</v>
       </c>
       <c r="D35">
-        <v>100</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -2357,7 +2357,7 @@
         <v>1</v>
       </c>
       <c r="D37">
-        <v>99.99990463256836</v>
+        <v>99.9997615814209</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -2368,7 +2368,7 @@
         <v>1</v>
       </c>
       <c r="D38">
-        <v>99.99984502792358</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -2390,7 +2390,7 @@
         <v>2</v>
       </c>
       <c r="D40">
-        <v>100</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -2434,7 +2434,7 @@
         <v>2</v>
       </c>
       <c r="D44">
-        <v>99.99997615814209</v>
+        <v>99.99994039535522</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -2467,7 +2467,7 @@
         <v>2</v>
       </c>
       <c r="D47">
-        <v>99.99771118164062</v>
+        <v>99.99994039535522</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -2489,7 +2489,7 @@
         <v>2</v>
       </c>
       <c r="D49">
-        <v>99.99150037765503</v>
+        <v>99.19838309288025</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -2522,7 +2522,7 @@
         <v>2</v>
       </c>
       <c r="D52">
-        <v>100</v>
+        <v>99.99995231628418</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -2555,7 +2555,7 @@
         <v>2</v>
       </c>
       <c r="D55">
-        <v>99.99991655349731</v>
+        <v>99.96691942214966</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -2588,7 +2588,7 @@
         <v>1</v>
       </c>
       <c r="D58">
-        <v>99.99990463256836</v>
+        <v>100</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -2610,7 +2610,7 @@
         <v>2</v>
       </c>
       <c r="D60">
-        <v>93.72910857200623</v>
+        <v>99.99130964279175</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -2632,7 +2632,7 @@
         <v>2</v>
       </c>
       <c r="D62">
-        <v>100</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -2643,7 +2643,7 @@
         <v>2</v>
       </c>
       <c r="D63">
-        <v>99.99998807907104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -2665,7 +2665,7 @@
         <v>2</v>
       </c>
       <c r="D65">
-        <v>99.9995231628418</v>
+        <v>99.99994039535522</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -2687,7 +2687,7 @@
         <v>2</v>
       </c>
       <c r="D67">
-        <v>99.20164346694946</v>
+        <v>99.98700618743896</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -2709,7 +2709,7 @@
         <v>2</v>
       </c>
       <c r="D69">
-        <v>99.99997615814209</v>
+        <v>100</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -2720,7 +2720,7 @@
         <v>2</v>
       </c>
       <c r="D70">
-        <v>96.93212509155273</v>
+        <v>99.99903440475464</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -2731,7 +2731,7 @@
         <v>2</v>
       </c>
       <c r="D71">
-        <v>99.99990463256836</v>
+        <v>100</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -2753,7 +2753,7 @@
         <v>2</v>
       </c>
       <c r="D73">
-        <v>99.67561364173889</v>
+        <v>70.98561525344849</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -2764,7 +2764,7 @@
         <v>2</v>
       </c>
       <c r="D74">
-        <v>99.99994039535522</v>
+        <v>100</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -2786,7 +2786,7 @@
         <v>2</v>
       </c>
       <c r="D76">
-        <v>100</v>
+        <v>99.9869704246521</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -2808,7 +2808,7 @@
         <v>2</v>
       </c>
       <c r="D78">
-        <v>99.99992847442627</v>
+        <v>100</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -2830,7 +2830,7 @@
         <v>2</v>
       </c>
       <c r="D80">
-        <v>100</v>
+        <v>99.99994039535522</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -2838,10 +2838,10 @@
         <v>82</v>
       </c>
       <c r="C81">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D81">
-        <v>99.99665021896362</v>
+        <v>100</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -2874,7 +2874,7 @@
         <v>2</v>
       </c>
       <c r="D84">
-        <v>99.99998807907104</v>
+        <v>99.99995231628418</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -2896,7 +2896,7 @@
         <v>1</v>
       </c>
       <c r="D86">
-        <v>64.58043456077576</v>
+        <v>99.99997615814209</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -2907,7 +2907,7 @@
         <v>2</v>
       </c>
       <c r="D87">
-        <v>99.99995231628418</v>
+        <v>100</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -2940,7 +2940,7 @@
         <v>2</v>
       </c>
       <c r="D90">
-        <v>99.99948740005493</v>
+        <v>100</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -2948,10 +2948,10 @@
         <v>92</v>
       </c>
       <c r="C91">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D91">
-        <v>99.99948740005493</v>
+        <v>99.94034767150879</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -2962,7 +2962,7 @@
         <v>2</v>
       </c>
       <c r="D92">
-        <v>99.99735355377197</v>
+        <v>56.22191429138184</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -3017,7 +3017,7 @@
         <v>2</v>
       </c>
       <c r="D97">
-        <v>99.99998807907104</v>
+        <v>93.39025616645813</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -3050,7 +3050,7 @@
         <v>1</v>
       </c>
       <c r="D100">
-        <v>99.99991655349731</v>
+        <v>99.99996423721313</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -3072,7 +3072,7 @@
         <v>1</v>
       </c>
       <c r="D102">
-        <v>100</v>
+        <v>99.99997615814209</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -3094,7 +3094,7 @@
         <v>2</v>
       </c>
       <c r="D104">
-        <v>100</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -3105,7 +3105,7 @@
         <v>2</v>
       </c>
       <c r="D105">
-        <v>99.99991655349731</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -3127,7 +3127,7 @@
         <v>2</v>
       </c>
       <c r="D107">
-        <v>100</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -3135,10 +3135,10 @@
         <v>109</v>
       </c>
       <c r="C108">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D108">
-        <v>99.57029223442078</v>
+        <v>99.99997615814209</v>
       </c>
     </row>
     <row r="109" spans="1:4">
@@ -3149,7 +3149,7 @@
         <v>1</v>
       </c>
       <c r="D109">
-        <v>100</v>
+        <v>99.99992847442627</v>
       </c>
     </row>
     <row r="110" spans="1:4">
@@ -3160,7 +3160,7 @@
         <v>1</v>
       </c>
       <c r="D110">
-        <v>99.99996423721313</v>
+        <v>100</v>
       </c>
     </row>
     <row r="111" spans="1:4">
@@ -3182,7 +3182,7 @@
         <v>1</v>
       </c>
       <c r="D112">
-        <v>99.99998807907104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="113" spans="1:4">
@@ -3193,7 +3193,7 @@
         <v>2</v>
       </c>
       <c r="D113">
-        <v>100</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="114" spans="1:4">
@@ -3226,7 +3226,7 @@
         <v>2</v>
       </c>
       <c r="D116">
-        <v>99.99998807907104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="117" spans="1:4">
@@ -3237,7 +3237,7 @@
         <v>2</v>
       </c>
       <c r="D117">
-        <v>99.99997615814209</v>
+        <v>100</v>
       </c>
     </row>
     <row r="118" spans="1:4">
@@ -3248,7 +3248,7 @@
         <v>2</v>
       </c>
       <c r="D118">
-        <v>99.99998807907104</v>
+        <v>95.69123983383179</v>
       </c>
     </row>
     <row r="119" spans="1:4">
@@ -3259,7 +3259,7 @@
         <v>2</v>
       </c>
       <c r="D119">
-        <v>100</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="120" spans="1:4">
@@ -3281,7 +3281,7 @@
         <v>2</v>
       </c>
       <c r="D121">
-        <v>99.99997615814209</v>
+        <v>100</v>
       </c>
     </row>
     <row r="122" spans="1:4">
@@ -3289,10 +3289,10 @@
         <v>123</v>
       </c>
       <c r="C122">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D122">
-        <v>88.72309327125549</v>
+        <v>99.99799728393555</v>
       </c>
     </row>
     <row r="123" spans="1:4">
@@ -3303,7 +3303,7 @@
         <v>2</v>
       </c>
       <c r="D123">
-        <v>97.74796366691589</v>
+        <v>99.9997615814209</v>
       </c>
     </row>
     <row r="124" spans="1:4">
@@ -3314,7 +3314,7 @@
         <v>2</v>
       </c>
       <c r="D124">
-        <v>99.99988079071045</v>
+        <v>100</v>
       </c>
     </row>
     <row r="125" spans="1:4">
@@ -3369,7 +3369,7 @@
         <v>2</v>
       </c>
       <c r="D129">
-        <v>99.99995231628418</v>
+        <v>100</v>
       </c>
     </row>
     <row r="130" spans="1:4">
@@ -3380,7 +3380,7 @@
         <v>2</v>
       </c>
       <c r="D130">
-        <v>100</v>
+        <v>99.99997615814209</v>
       </c>
     </row>
     <row r="131" spans="1:4">
@@ -3413,7 +3413,7 @@
         <v>2</v>
       </c>
       <c r="D133">
-        <v>99.99997615814209</v>
+        <v>100</v>
       </c>
     </row>
     <row r="134" spans="1:4">
@@ -3424,7 +3424,7 @@
         <v>2</v>
       </c>
       <c r="D134">
-        <v>99.99998807907104</v>
+        <v>99.99918937683105</v>
       </c>
     </row>
     <row r="135" spans="1:4">
@@ -3432,10 +3432,10 @@
         <v>136</v>
       </c>
       <c r="C135">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D135">
-        <v>100</v>
+        <v>99.99823570251465</v>
       </c>
     </row>
     <row r="136" spans="1:4">
@@ -3523,7 +3523,7 @@
         <v>2</v>
       </c>
       <c r="D143">
-        <v>99.99998807907104</v>
+        <v>99.99995231628418</v>
       </c>
     </row>
     <row r="144" spans="1:4">
@@ -3534,7 +3534,7 @@
         <v>2</v>
       </c>
       <c r="D144">
-        <v>99.99985694885254</v>
+        <v>97.9665219783783</v>
       </c>
     </row>
     <row r="145" spans="1:4">
@@ -3545,7 +3545,7 @@
         <v>2</v>
       </c>
       <c r="D145">
-        <v>99.99994039535522</v>
+        <v>99.99914169311523</v>
       </c>
     </row>
     <row r="146" spans="1:4">
@@ -3556,7 +3556,7 @@
         <v>1</v>
       </c>
       <c r="D146">
-        <v>99.99959468841553</v>
+        <v>99.99979734420776</v>
       </c>
     </row>
     <row r="147" spans="1:4">
@@ -3564,10 +3564,10 @@
         <v>148</v>
       </c>
       <c r="C147">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D147">
-        <v>99.99983310699463</v>
+        <v>98.94521236419678</v>
       </c>
     </row>
     <row r="148" spans="1:4">
@@ -3600,7 +3600,7 @@
         <v>2</v>
       </c>
       <c r="D150">
-        <v>99.9998927116394</v>
+        <v>100</v>
       </c>
     </row>
     <row r="151" spans="1:4">
@@ -3655,7 +3655,7 @@
         <v>1</v>
       </c>
       <c r="D155">
-        <v>99.99997615814209</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="156" spans="1:4">
@@ -3677,7 +3677,7 @@
         <v>2</v>
       </c>
       <c r="D157">
-        <v>100</v>
+        <v>99.99996423721313</v>
       </c>
     </row>
     <row r="158" spans="1:4">
@@ -3696,10 +3696,10 @@
         <v>160</v>
       </c>
       <c r="C159">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D159">
-        <v>100</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="160" spans="1:4">
@@ -3743,7 +3743,7 @@
         <v>2</v>
       </c>
       <c r="D163">
-        <v>99.99971389770508</v>
+        <v>99.99967813491821</v>
       </c>
     </row>
     <row r="164" spans="1:4">
@@ -3754,7 +3754,7 @@
         <v>2</v>
       </c>
       <c r="D164">
-        <v>99.99971389770508</v>
+        <v>99.99967813491821</v>
       </c>
     </row>
     <row r="165" spans="1:4">
@@ -3765,7 +3765,7 @@
         <v>2</v>
       </c>
       <c r="D165">
-        <v>99.99998807907104</v>
+        <v>99.99990463256836</v>
       </c>
     </row>
     <row r="166" spans="1:4">
@@ -3787,7 +3787,7 @@
         <v>1</v>
       </c>
       <c r="D167">
-        <v>99.99892711639404</v>
+        <v>98.89899492263794</v>
       </c>
     </row>
     <row r="168" spans="1:4">
@@ -3820,7 +3820,7 @@
         <v>2</v>
       </c>
       <c r="D170">
-        <v>99.99924898147583</v>
+        <v>99.99414682388306</v>
       </c>
     </row>
     <row r="171" spans="1:4">
@@ -3842,7 +3842,7 @@
         <v>2</v>
       </c>
       <c r="D172">
-        <v>99.99998807907104</v>
+        <v>99.99997615814209</v>
       </c>
     </row>
     <row r="173" spans="1:4">
@@ -3853,7 +3853,7 @@
         <v>2</v>
       </c>
       <c r="D173">
-        <v>99.99990463256836</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="174" spans="1:4">
@@ -3919,7 +3919,7 @@
         <v>2</v>
       </c>
       <c r="D179">
-        <v>100</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="180" spans="1:4">
@@ -3930,7 +3930,7 @@
         <v>2</v>
       </c>
       <c r="D180">
-        <v>99.99998807907104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="181" spans="1:4">
@@ -3941,7 +3941,7 @@
         <v>2</v>
       </c>
       <c r="D181">
-        <v>99.99985694885254</v>
+        <v>95.89575529098511</v>
       </c>
     </row>
     <row r="182" spans="1:4">
@@ -4040,7 +4040,7 @@
         <v>1</v>
       </c>
       <c r="D190">
-        <v>99.99480247497559</v>
+        <v>61.68338656425476</v>
       </c>
     </row>
     <row r="191" spans="1:4">
@@ -4051,7 +4051,7 @@
         <v>2</v>
       </c>
       <c r="D191">
-        <v>99.95464682579041</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="192" spans="1:4">
@@ -4062,7 +4062,7 @@
         <v>2</v>
       </c>
       <c r="D192">
-        <v>99.99997615814209</v>
+        <v>100</v>
       </c>
     </row>
     <row r="193" spans="1:4">
@@ -4095,7 +4095,7 @@
         <v>2</v>
       </c>
       <c r="D195">
-        <v>99.99991655349731</v>
+        <v>100</v>
       </c>
     </row>
     <row r="196" spans="1:4">
@@ -4106,7 +4106,7 @@
         <v>2</v>
       </c>
       <c r="D196">
-        <v>99.99997615814209</v>
+        <v>100</v>
       </c>
     </row>
     <row r="197" spans="1:4">
@@ -4117,7 +4117,7 @@
         <v>2</v>
       </c>
       <c r="D197">
-        <v>99.99387264251709</v>
+        <v>99.98842477798462</v>
       </c>
     </row>
     <row r="198" spans="1:4">
@@ -4128,7 +4128,7 @@
         <v>2</v>
       </c>
       <c r="D198">
-        <v>99.99997615814209</v>
+        <v>99.99990463256836</v>
       </c>
     </row>
     <row r="199" spans="1:4">
@@ -4139,7 +4139,7 @@
         <v>2</v>
       </c>
       <c r="D199">
-        <v>99.99979734420776</v>
+        <v>99.99958276748657</v>
       </c>
     </row>
     <row r="200" spans="1:4">
@@ -4150,7 +4150,7 @@
         <v>2</v>
       </c>
       <c r="D200">
-        <v>100</v>
+        <v>75.19803047180176</v>
       </c>
     </row>
     <row r="201" spans="1:4">
@@ -4183,7 +4183,7 @@
         <v>2</v>
       </c>
       <c r="D203">
-        <v>99.99998807907104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="204" spans="1:4">
@@ -4194,7 +4194,7 @@
         <v>2</v>
       </c>
       <c r="D204">
-        <v>99.99998807907104</v>
+        <v>99.99997615814209</v>
       </c>
     </row>
     <row r="205" spans="1:4">
@@ -4205,7 +4205,7 @@
         <v>2</v>
       </c>
       <c r="D205">
-        <v>99.99846220016479</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="206" spans="1:4">
@@ -4213,10 +4213,10 @@
         <v>206</v>
       </c>
       <c r="C206">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D206">
-        <v>99.9987006187439</v>
+        <v>99.9994158744812</v>
       </c>
     </row>
     <row r="207" spans="1:4">
@@ -4227,7 +4227,7 @@
         <v>2</v>
       </c>
       <c r="D207">
-        <v>100</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="208" spans="1:4">
@@ -4249,7 +4249,7 @@
         <v>2</v>
       </c>
       <c r="D209">
-        <v>99.99984502792358</v>
+        <v>99.99841451644897</v>
       </c>
     </row>
     <row r="210" spans="1:4">
@@ -4260,7 +4260,7 @@
         <v>2</v>
       </c>
       <c r="D210">
-        <v>99.99992847442627</v>
+        <v>99.99909400939941</v>
       </c>
     </row>
     <row r="211" spans="1:4">
@@ -4271,7 +4271,7 @@
         <v>2</v>
       </c>
       <c r="D211">
-        <v>99.99971389770508</v>
+        <v>99.83751773834229</v>
       </c>
     </row>
     <row r="212" spans="1:4">
@@ -4282,7 +4282,7 @@
         <v>2</v>
       </c>
       <c r="D212">
-        <v>99.99974966049194</v>
+        <v>100</v>
       </c>
     </row>
     <row r="213" spans="1:4">
@@ -4293,7 +4293,7 @@
         <v>2</v>
       </c>
       <c r="D213">
-        <v>99.99998807907104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="214" spans="1:4">
@@ -4304,7 +4304,7 @@
         <v>2</v>
       </c>
       <c r="D214">
-        <v>100</v>
+        <v>99.99430179595947</v>
       </c>
     </row>
     <row r="215" spans="1:4">
@@ -4315,7 +4315,7 @@
         <v>2</v>
       </c>
       <c r="D215">
-        <v>99.99986886978149</v>
+        <v>90.5474841594696</v>
       </c>
     </row>
     <row r="216" spans="1:4">
@@ -4326,7 +4326,7 @@
         <v>2</v>
       </c>
       <c r="D216">
-        <v>99.99997615814209</v>
+        <v>86.62658333778381</v>
       </c>
     </row>
     <row r="217" spans="1:4">
@@ -4337,7 +4337,7 @@
         <v>2</v>
       </c>
       <c r="D217">
-        <v>99.99998807907104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="218" spans="1:4">
@@ -4348,7 +4348,7 @@
         <v>2</v>
       </c>
       <c r="D218">
-        <v>100</v>
+        <v>99.99995231628418</v>
       </c>
     </row>
     <row r="219" spans="1:4">
@@ -4356,10 +4356,10 @@
         <v>219</v>
       </c>
       <c r="C219">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D219">
-        <v>85.5742871761322</v>
+        <v>99.99955892562866</v>
       </c>
     </row>
     <row r="220" spans="1:4">
@@ -4370,7 +4370,7 @@
         <v>2</v>
       </c>
       <c r="D220">
-        <v>100</v>
+        <v>99.99997615814209</v>
       </c>
     </row>
     <row r="221" spans="1:4">
@@ -4381,7 +4381,7 @@
         <v>2</v>
       </c>
       <c r="D221">
-        <v>99.99996423721313</v>
+        <v>99.99995231628418</v>
       </c>
     </row>
     <row r="222" spans="1:4">
@@ -4414,7 +4414,7 @@
         <v>2</v>
       </c>
       <c r="D224">
-        <v>99.99997615814209</v>
+        <v>100</v>
       </c>
     </row>
     <row r="225" spans="1:4">
@@ -4436,7 +4436,7 @@
         <v>2</v>
       </c>
       <c r="D226">
-        <v>87.87776827812195</v>
+        <v>99.99842643737793</v>
       </c>
     </row>
     <row r="227" spans="1:4">
@@ -4447,7 +4447,7 @@
         <v>1</v>
       </c>
       <c r="D227">
-        <v>99.99997615814209</v>
+        <v>100</v>
       </c>
     </row>
     <row r="228" spans="1:4">
@@ -4491,7 +4491,7 @@
         <v>2</v>
       </c>
       <c r="D231">
-        <v>99.99998807907104</v>
+        <v>92.84529685974121</v>
       </c>
     </row>
     <row r="232" spans="1:4">
@@ -4502,7 +4502,7 @@
         <v>2</v>
       </c>
       <c r="D232">
-        <v>100</v>
+        <v>99.98948574066162</v>
       </c>
     </row>
     <row r="233" spans="1:4">
@@ -4513,7 +4513,7 @@
         <v>2</v>
       </c>
       <c r="D233">
-        <v>99.99998807907104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="234" spans="1:4">
@@ -4524,7 +4524,7 @@
         <v>2</v>
       </c>
       <c r="D234">
-        <v>99.99996423721313</v>
+        <v>99.99938011169434</v>
       </c>
     </row>
     <row r="235" spans="1:4">
@@ -4546,7 +4546,7 @@
         <v>1</v>
       </c>
       <c r="D236">
-        <v>99.99998807907104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="237" spans="1:4">
@@ -4590,7 +4590,7 @@
         <v>2</v>
       </c>
       <c r="D240">
-        <v>99.99699592590332</v>
+        <v>99.68312382698059</v>
       </c>
     </row>
     <row r="241" spans="1:4">
@@ -4601,7 +4601,7 @@
         <v>2</v>
       </c>
       <c r="D241">
-        <v>99.99901056289673</v>
+        <v>99.9988317489624</v>
       </c>
     </row>
     <row r="242" spans="1:4">
@@ -4612,7 +4612,7 @@
         <v>2</v>
       </c>
       <c r="D242">
-        <v>99.99998807907104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="243" spans="1:4">
@@ -4623,7 +4623,7 @@
         <v>2</v>
       </c>
       <c r="D243">
-        <v>99.99685287475586</v>
+        <v>99.99977350234985</v>
       </c>
     </row>
     <row r="244" spans="1:4">
@@ -4634,7 +4634,7 @@
         <v>2</v>
       </c>
       <c r="D244">
-        <v>100</v>
+        <v>99.99994039535522</v>
       </c>
     </row>
     <row r="245" spans="1:4">
@@ -4656,7 +4656,7 @@
         <v>2</v>
       </c>
       <c r="D246">
-        <v>99.99998807907104</v>
+        <v>99.99409914016724</v>
       </c>
     </row>
     <row r="247" spans="1:4">
@@ -4667,7 +4667,7 @@
         <v>2</v>
       </c>
       <c r="D247">
-        <v>99.99982118606567</v>
+        <v>51.28035545349121</v>
       </c>
     </row>
     <row r="248" spans="1:4">
@@ -4678,7 +4678,7 @@
         <v>2</v>
       </c>
       <c r="D248">
-        <v>99.99982118606567</v>
+        <v>100</v>
       </c>
     </row>
     <row r="249" spans="1:4">
@@ -4700,7 +4700,7 @@
         <v>2</v>
       </c>
       <c r="D250">
-        <v>99.99921321868896</v>
+        <v>100</v>
       </c>
     </row>
     <row r="251" spans="1:4">
@@ -4711,7 +4711,7 @@
         <v>2</v>
       </c>
       <c r="D251">
-        <v>100</v>
+        <v>99.99996423721313</v>
       </c>
     </row>
     <row r="252" spans="1:4">
@@ -4722,7 +4722,7 @@
         <v>2</v>
       </c>
       <c r="D252">
-        <v>99.9819815158844</v>
+        <v>99.96945858001709</v>
       </c>
     </row>
     <row r="253" spans="1:4">
@@ -4733,7 +4733,7 @@
         <v>2</v>
       </c>
       <c r="D253">
-        <v>99.99809265136719</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="254" spans="1:4">
@@ -4744,7 +4744,7 @@
         <v>2</v>
       </c>
       <c r="D254">
-        <v>100</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="255" spans="1:4">
@@ -4755,7 +4755,7 @@
         <v>2</v>
       </c>
       <c r="D255">
-        <v>99.99997615814209</v>
+        <v>99.99665021896362</v>
       </c>
     </row>
     <row r="256" spans="1:4">
@@ -4766,7 +4766,7 @@
         <v>2</v>
       </c>
       <c r="D256">
-        <v>99.9819815158844</v>
+        <v>99.96945858001709</v>
       </c>
     </row>
     <row r="257" spans="1:4">
@@ -4777,7 +4777,7 @@
         <v>2</v>
       </c>
       <c r="D257">
-        <v>99.9997615814209</v>
+        <v>99.99890327453613</v>
       </c>
     </row>
     <row r="258" spans="1:4">
@@ -4788,7 +4788,7 @@
         <v>2</v>
       </c>
       <c r="D258">
-        <v>99.99982118606567</v>
+        <v>99.9997615814209</v>
       </c>
     </row>
     <row r="259" spans="1:4">
@@ -4799,7 +4799,7 @@
         <v>2</v>
       </c>
       <c r="D259">
-        <v>99.99997615814209</v>
+        <v>100</v>
       </c>
     </row>
     <row r="260" spans="1:4">
@@ -4821,7 +4821,7 @@
         <v>2</v>
       </c>
       <c r="D261">
-        <v>99.99994039535522</v>
+        <v>100</v>
       </c>
     </row>
     <row r="262" spans="1:4">
@@ -4832,7 +4832,7 @@
         <v>2</v>
       </c>
       <c r="D262">
-        <v>99.99998807907104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="263" spans="1:4">
@@ -4854,7 +4854,7 @@
         <v>2</v>
       </c>
       <c r="D264">
-        <v>99.99997615814209</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="265" spans="1:4">
@@ -4876,7 +4876,7 @@
         <v>2</v>
       </c>
       <c r="D266">
-        <v>99.99998807907104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="267" spans="1:4">
@@ -4887,7 +4887,7 @@
         <v>2</v>
       </c>
       <c r="D267">
-        <v>100</v>
+        <v>99.99996423721313</v>
       </c>
     </row>
     <row r="268" spans="1:4">
@@ -4895,10 +4895,10 @@
         <v>267</v>
       </c>
       <c r="C268">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D268">
-        <v>99.37799572944641</v>
+        <v>99.99973773956299</v>
       </c>
     </row>
     <row r="269" spans="1:4">
@@ -4909,7 +4909,7 @@
         <v>2</v>
       </c>
       <c r="D269">
-        <v>99.99996423721313</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="270" spans="1:4">
@@ -4953,7 +4953,7 @@
         <v>2</v>
       </c>
       <c r="D273">
-        <v>99.99585151672363</v>
+        <v>100</v>
       </c>
     </row>
     <row r="274" spans="1:4">
@@ -4964,7 +4964,7 @@
         <v>2</v>
       </c>
       <c r="D274">
-        <v>99.99998807907104</v>
+        <v>99.98890161514282</v>
       </c>
     </row>
     <row r="275" spans="1:4">
@@ -4975,7 +4975,7 @@
         <v>1</v>
       </c>
       <c r="D275">
-        <v>99.99974966049194</v>
+        <v>99.99995231628418</v>
       </c>
     </row>
     <row r="276" spans="1:4">
@@ -4986,7 +4986,7 @@
         <v>2</v>
       </c>
       <c r="D276">
-        <v>100</v>
+        <v>74.10802841186523</v>
       </c>
     </row>
     <row r="277" spans="1:4">
@@ -5005,10 +5005,10 @@
         <v>277</v>
       </c>
       <c r="C278">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D278">
-        <v>99.99971389770508</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="279" spans="1:4">
@@ -5019,7 +5019,7 @@
         <v>2</v>
       </c>
       <c r="D279">
-        <v>99.99977350234985</v>
+        <v>99.99996423721313</v>
       </c>
     </row>
     <row r="280" spans="1:4">
@@ -5030,7 +5030,7 @@
         <v>2</v>
       </c>
       <c r="D280">
-        <v>99.99990463256836</v>
+        <v>99.99971389770508</v>
       </c>
     </row>
     <row r="281" spans="1:4">
@@ -5096,7 +5096,7 @@
         <v>2</v>
       </c>
       <c r="D286">
-        <v>99.00930523872375</v>
+        <v>99.99388456344604</v>
       </c>
     </row>
     <row r="287" spans="1:4">
@@ -5118,7 +5118,7 @@
         <v>2</v>
       </c>
       <c r="D288">
-        <v>99.9995231628418</v>
+        <v>99.99994039535522</v>
       </c>
     </row>
     <row r="289" spans="1:4">
@@ -5140,7 +5140,7 @@
         <v>2</v>
       </c>
       <c r="D290">
-        <v>99.99992847442627</v>
+        <v>99.99997615814209</v>
       </c>
     </row>
     <row r="291" spans="1:4">
@@ -5151,7 +5151,7 @@
         <v>2</v>
       </c>
       <c r="D291">
-        <v>99.99995231628418</v>
+        <v>100</v>
       </c>
     </row>
     <row r="292" spans="1:4">
@@ -5162,7 +5162,7 @@
         <v>2</v>
       </c>
       <c r="D292">
-        <v>99.99995231628418</v>
+        <v>99.9998927116394</v>
       </c>
     </row>
     <row r="293" spans="1:4">
@@ -5173,7 +5173,7 @@
         <v>2</v>
       </c>
       <c r="D293">
-        <v>99.99867677688599</v>
+        <v>100</v>
       </c>
     </row>
     <row r="294" spans="1:4">
@@ -5184,7 +5184,7 @@
         <v>2</v>
       </c>
       <c r="D294">
-        <v>100</v>
+        <v>99.99920129776001</v>
       </c>
     </row>
     <row r="295" spans="1:4">
@@ -5195,7 +5195,7 @@
         <v>2</v>
       </c>
       <c r="D295">
-        <v>99.99951124191284</v>
+        <v>99.79878664016724</v>
       </c>
     </row>
     <row r="296" spans="1:4">
@@ -5203,10 +5203,10 @@
         <v>294</v>
       </c>
       <c r="C296">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D296">
-        <v>99.99774694442749</v>
+        <v>99.80815649032593</v>
       </c>
     </row>
     <row r="297" spans="1:4">
@@ -5217,7 +5217,7 @@
         <v>2</v>
       </c>
       <c r="D297">
-        <v>99.99955892562866</v>
+        <v>99.99997615814209</v>
       </c>
     </row>
     <row r="298" spans="1:4">
@@ -5228,7 +5228,7 @@
         <v>2</v>
       </c>
       <c r="D298">
-        <v>99.99978542327881</v>
+        <v>99.99983310699463</v>
       </c>
     </row>
     <row r="299" spans="1:4">
@@ -5250,7 +5250,7 @@
         <v>1</v>
       </c>
       <c r="D300">
-        <v>99.99998807907104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="301" spans="1:4">
@@ -5272,7 +5272,7 @@
         <v>2</v>
       </c>
       <c r="D302">
-        <v>99.99997615814209</v>
+        <v>100</v>
       </c>
     </row>
     <row r="303" spans="1:4">
@@ -5280,10 +5280,10 @@
         <v>301</v>
       </c>
       <c r="C303">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D303">
-        <v>99.99977350234985</v>
+        <v>95.96152305603027</v>
       </c>
     </row>
     <row r="304" spans="1:4">
@@ -5294,7 +5294,7 @@
         <v>2</v>
       </c>
       <c r="D304">
-        <v>99.99458789825439</v>
+        <v>99.99650716781616</v>
       </c>
     </row>
     <row r="305" spans="1:4">
@@ -5305,7 +5305,7 @@
         <v>1</v>
       </c>
       <c r="D305">
-        <v>99.99980926513672</v>
+        <v>99.99995231628418</v>
       </c>
     </row>
     <row r="306" spans="1:4">
@@ -5316,7 +5316,7 @@
         <v>2</v>
       </c>
       <c r="D306">
-        <v>97.97767996788025</v>
+        <v>99.99997615814209</v>
       </c>
     </row>
     <row r="307" spans="1:4">
@@ -5338,7 +5338,7 @@
         <v>1</v>
       </c>
       <c r="D308">
-        <v>99.99985694885254</v>
+        <v>99.99921321868896</v>
       </c>
     </row>
     <row r="309" spans="1:4">
@@ -5346,10 +5346,10 @@
         <v>307</v>
       </c>
       <c r="C309">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D309">
-        <v>99.99943971633911</v>
+        <v>99.99995231628418</v>
       </c>
     </row>
     <row r="310" spans="1:4">
@@ -5371,7 +5371,7 @@
         <v>2</v>
       </c>
       <c r="D311">
-        <v>99.99969005584717</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="312" spans="1:4">
@@ -5393,7 +5393,7 @@
         <v>2</v>
       </c>
       <c r="D313">
-        <v>99.99992847442627</v>
+        <v>99.99997615814209</v>
       </c>
     </row>
     <row r="314" spans="1:4">
@@ -5401,10 +5401,10 @@
         <v>312</v>
       </c>
       <c r="C314">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D314">
-        <v>99.99628067016602</v>
+        <v>99.9749481678009</v>
       </c>
     </row>
     <row r="315" spans="1:4">
@@ -5434,10 +5434,10 @@
         <v>315</v>
       </c>
       <c r="C317">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D317">
-        <v>99.92473125457764</v>
+        <v>97.58703708648682</v>
       </c>
     </row>
     <row r="318" spans="1:4">
@@ -5448,7 +5448,7 @@
         <v>2</v>
       </c>
       <c r="D318">
-        <v>99.99998807907104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="319" spans="1:4">
@@ -5467,10 +5467,10 @@
         <v>219</v>
       </c>
       <c r="C320">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D320">
-        <v>85.5742871761322</v>
+        <v>99.99955892562866</v>
       </c>
     </row>
     <row r="321" spans="1:4">
@@ -5503,7 +5503,7 @@
         <v>1</v>
       </c>
       <c r="D323">
-        <v>69.7151243686676</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="324" spans="1:4">
@@ -5514,7 +5514,7 @@
         <v>1</v>
       </c>
       <c r="D324">
-        <v>100</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="325" spans="1:4">
@@ -5525,7 +5525,7 @@
         <v>1</v>
       </c>
       <c r="D325">
-        <v>100</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="326" spans="1:4">
@@ -5547,7 +5547,7 @@
         <v>2</v>
       </c>
       <c r="D327">
-        <v>99.99997615814209</v>
+        <v>99.99990463256836</v>
       </c>
     </row>
     <row r="328" spans="1:4">
@@ -5558,7 +5558,7 @@
         <v>2</v>
       </c>
       <c r="D328">
-        <v>99.99996423721313</v>
+        <v>99.99990463256836</v>
       </c>
     </row>
     <row r="329" spans="1:4">
@@ -5580,7 +5580,7 @@
         <v>2</v>
       </c>
       <c r="D330">
-        <v>99.9998927116394</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="331" spans="1:4">
@@ -5602,7 +5602,7 @@
         <v>2</v>
       </c>
       <c r="D332">
-        <v>99.99995231628418</v>
+        <v>99.99836683273315</v>
       </c>
     </row>
     <row r="333" spans="1:4">
@@ -5613,7 +5613,7 @@
         <v>2</v>
       </c>
       <c r="D333">
-        <v>99.99998807907104</v>
+        <v>99.99994039535522</v>
       </c>
     </row>
     <row r="334" spans="1:4">
@@ -5624,7 +5624,7 @@
         <v>2</v>
       </c>
       <c r="D334">
-        <v>99.99992847442627</v>
+        <v>99.99994039535522</v>
       </c>
     </row>
     <row r="335" spans="1:4">
@@ -5635,7 +5635,7 @@
         <v>2</v>
       </c>
       <c r="D335">
-        <v>99.99998807907104</v>
+        <v>99.99997615814209</v>
       </c>
     </row>
     <row r="336" spans="1:4">
@@ -5646,7 +5646,7 @@
         <v>2</v>
       </c>
       <c r="D336">
-        <v>99.99998807907104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="337" spans="1:4">
@@ -5679,7 +5679,7 @@
         <v>2</v>
       </c>
       <c r="D339">
-        <v>99.99992847442627</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="340" spans="1:4">
@@ -5687,10 +5687,10 @@
         <v>336</v>
       </c>
       <c r="C340">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D340">
-        <v>100</v>
+        <v>99.99655485153198</v>
       </c>
     </row>
     <row r="341" spans="1:4">
@@ -5701,7 +5701,7 @@
         <v>2</v>
       </c>
       <c r="D341">
-        <v>99.9997615814209</v>
+        <v>100</v>
       </c>
     </row>
     <row r="342" spans="1:4">
@@ -5709,10 +5709,10 @@
         <v>338</v>
       </c>
       <c r="C342">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D342">
-        <v>99.99586343765259</v>
+        <v>99.99971389770508</v>
       </c>
     </row>
     <row r="343" spans="1:4">
@@ -5753,10 +5753,10 @@
         <v>342</v>
       </c>
       <c r="C346">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D346">
-        <v>99.99504089355469</v>
+        <v>99.91728663444519</v>
       </c>
     </row>
     <row r="347" spans="1:4">
@@ -5767,7 +5767,7 @@
         <v>2</v>
       </c>
       <c r="D347">
-        <v>99.99904632568359</v>
+        <v>99.99812841415405</v>
       </c>
     </row>
     <row r="348" spans="1:4">
@@ -5778,7 +5778,7 @@
         <v>1</v>
       </c>
       <c r="D348">
-        <v>100</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="349" spans="1:4">
@@ -5789,7 +5789,7 @@
         <v>2</v>
       </c>
       <c r="D349">
-        <v>99.99948740005493</v>
+        <v>99.99996423721313</v>
       </c>
     </row>
     <row r="350" spans="1:4">
@@ -5800,7 +5800,7 @@
         <v>2</v>
       </c>
       <c r="D350">
-        <v>100</v>
+        <v>98.3357846736908</v>
       </c>
     </row>
     <row r="351" spans="1:4">
@@ -5808,10 +5808,10 @@
         <v>347</v>
       </c>
       <c r="C351">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D351">
-        <v>99.99198913574219</v>
+        <v>99.99171495437622</v>
       </c>
     </row>
     <row r="352" spans="1:4">
@@ -5822,7 +5822,7 @@
         <v>2</v>
       </c>
       <c r="D352">
-        <v>99.99992847442627</v>
+        <v>99.99909400939941</v>
       </c>
     </row>
     <row r="353" spans="1:4">
@@ -5833,7 +5833,7 @@
         <v>2</v>
       </c>
       <c r="D353">
-        <v>100</v>
+        <v>99.99793767929077</v>
       </c>
     </row>
     <row r="354" spans="1:4">
@@ -5855,7 +5855,7 @@
         <v>2</v>
       </c>
       <c r="D355">
-        <v>98.50153923034668</v>
+        <v>99.95741248130798</v>
       </c>
     </row>
     <row r="356" spans="1:4">
@@ -5866,7 +5866,7 @@
         <v>1</v>
       </c>
       <c r="D356">
-        <v>99.99992847442627</v>
+        <v>99.99986886978149</v>
       </c>
     </row>
     <row r="357" spans="1:4">
@@ -5877,7 +5877,7 @@
         <v>1</v>
       </c>
       <c r="D357">
-        <v>99.99995231628418</v>
+        <v>99.99994039535522</v>
       </c>
     </row>
     <row r="358" spans="1:4">
@@ -5888,7 +5888,7 @@
         <v>1</v>
       </c>
       <c r="D358">
-        <v>99.99998807907104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="359" spans="1:4">
@@ -5899,7 +5899,7 @@
         <v>1</v>
       </c>
       <c r="D359">
-        <v>99.99996423721313</v>
+        <v>99.99991655349731</v>
       </c>
     </row>
     <row r="360" spans="1:4">
@@ -5910,7 +5910,7 @@
         <v>2</v>
       </c>
       <c r="D360">
-        <v>99.99997615814209</v>
+        <v>100</v>
       </c>
     </row>
     <row r="361" spans="1:4">
@@ -5943,7 +5943,7 @@
         <v>2</v>
       </c>
       <c r="D363">
-        <v>99.99701976776123</v>
+        <v>99.56061244010925</v>
       </c>
     </row>
     <row r="364" spans="1:4">
@@ -5954,7 +5954,7 @@
         <v>2</v>
       </c>
       <c r="D364">
-        <v>100</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="365" spans="1:4">
@@ -5976,7 +5976,7 @@
         <v>2</v>
       </c>
       <c r="D366">
-        <v>99.99812841415405</v>
+        <v>100</v>
       </c>
     </row>
     <row r="367" spans="1:4">
@@ -5995,10 +5995,10 @@
         <v>363</v>
       </c>
       <c r="C368">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D368">
-        <v>57.43600726127625</v>
+        <v>99.74391460418701</v>
       </c>
     </row>
     <row r="369" spans="1:4">
@@ -6017,10 +6017,10 @@
         <v>365</v>
       </c>
       <c r="C370">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D370">
-        <v>53.59863042831421</v>
+        <v>99.99994039535522</v>
       </c>
     </row>
     <row r="371" spans="1:4">
@@ -6031,7 +6031,7 @@
         <v>2</v>
       </c>
       <c r="D371">
-        <v>99.99998807907104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="372" spans="1:4">
@@ -6053,7 +6053,7 @@
         <v>1</v>
       </c>
       <c r="D373">
-        <v>99.99998807907104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="374" spans="1:4">
@@ -6061,10 +6061,10 @@
         <v>369</v>
       </c>
       <c r="C374">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D374">
-        <v>99.99973773956299</v>
+        <v>99.99995231628418</v>
       </c>
     </row>
     <row r="375" spans="1:4">
@@ -6075,7 +6075,7 @@
         <v>2</v>
       </c>
       <c r="D375">
-        <v>99.99998807907104</v>
+        <v>79.8502504825592</v>
       </c>
     </row>
     <row r="376" spans="1:4">
@@ -6086,7 +6086,7 @@
         <v>2</v>
       </c>
       <c r="D376">
-        <v>99.99921321868896</v>
+        <v>99.94497895240784</v>
       </c>
     </row>
     <row r="377" spans="1:4">
@@ -6108,7 +6108,7 @@
         <v>2</v>
       </c>
       <c r="D378">
-        <v>99.99997615814209</v>
+        <v>85.15888452529907</v>
       </c>
     </row>
     <row r="379" spans="1:4">
@@ -6119,7 +6119,7 @@
         <v>2</v>
       </c>
       <c r="D379">
-        <v>100</v>
+        <v>99.99921321868896</v>
       </c>
     </row>
     <row r="380" spans="1:4">
@@ -6130,7 +6130,7 @@
         <v>2</v>
       </c>
       <c r="D380">
-        <v>99.99997615814209</v>
+        <v>100</v>
       </c>
     </row>
     <row r="381" spans="1:4">
@@ -6141,7 +6141,7 @@
         <v>1</v>
       </c>
       <c r="D381">
-        <v>99.7986912727356</v>
+        <v>67.32175946235657</v>
       </c>
     </row>
     <row r="382" spans="1:4">
@@ -6207,7 +6207,7 @@
         <v>2</v>
       </c>
       <c r="D387">
-        <v>99.9819815158844</v>
+        <v>99.96945858001709</v>
       </c>
     </row>
     <row r="388" spans="1:4">
@@ -6218,7 +6218,7 @@
         <v>2</v>
       </c>
       <c r="D388">
-        <v>99.99995231628418</v>
+        <v>99.99997615814209</v>
       </c>
     </row>
     <row r="389" spans="1:4">
@@ -6229,7 +6229,7 @@
         <v>2</v>
       </c>
       <c r="D389">
-        <v>100</v>
+        <v>99.99959468841553</v>
       </c>
     </row>
     <row r="390" spans="1:4">
@@ -6240,7 +6240,7 @@
         <v>2</v>
       </c>
       <c r="D390">
-        <v>99.99997615814209</v>
+        <v>99.85727071762085</v>
       </c>
     </row>
     <row r="391" spans="1:4">
@@ -6251,7 +6251,7 @@
         <v>1</v>
       </c>
       <c r="D391">
-        <v>99.99998807907104</v>
+        <v>99.99986886978149</v>
       </c>
     </row>
     <row r="392" spans="1:4">
@@ -6262,7 +6262,7 @@
         <v>1</v>
       </c>
       <c r="D392">
-        <v>100</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="393" spans="1:4">
@@ -6270,10 +6270,10 @@
         <v>387</v>
       </c>
       <c r="C393">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D393">
-        <v>99.99995231628418</v>
+        <v>100</v>
       </c>
     </row>
     <row r="394" spans="1:4">
@@ -6295,7 +6295,7 @@
         <v>2</v>
       </c>
       <c r="D395">
-        <v>100</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="396" spans="1:4">
@@ -6306,7 +6306,7 @@
         <v>2</v>
       </c>
       <c r="D396">
-        <v>99.98303651809692</v>
+        <v>100</v>
       </c>
     </row>
     <row r="397" spans="1:4">
@@ -6328,7 +6328,7 @@
         <v>2</v>
       </c>
       <c r="D398">
-        <v>99.99995231628418</v>
+        <v>100</v>
       </c>
     </row>
     <row r="399" spans="1:4">
@@ -6383,7 +6383,7 @@
         <v>2</v>
       </c>
       <c r="D403">
-        <v>100</v>
+        <v>99.99996423721313</v>
       </c>
     </row>
     <row r="404" spans="1:4">
@@ -6394,7 +6394,7 @@
         <v>2</v>
       </c>
       <c r="D404">
-        <v>99.99990463256836</v>
+        <v>99.9992847442627</v>
       </c>
     </row>
     <row r="405" spans="1:4">
@@ -6449,7 +6449,7 @@
         <v>2</v>
       </c>
       <c r="D409">
-        <v>99.99942779541016</v>
+        <v>99.99467134475708</v>
       </c>
     </row>
     <row r="410" spans="1:4">
@@ -6471,7 +6471,7 @@
         <v>1</v>
       </c>
       <c r="D411">
-        <v>99.99995231628418</v>
+        <v>100</v>
       </c>
     </row>
     <row r="412" spans="1:4">
@@ -6490,10 +6490,10 @@
         <v>407</v>
       </c>
       <c r="C413">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D413">
-        <v>99.99972581863403</v>
+        <v>99.99921321868896</v>
       </c>
     </row>
     <row r="414" spans="1:4">
@@ -6501,10 +6501,10 @@
         <v>408</v>
       </c>
       <c r="C414">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D414">
-        <v>99.99136924743652</v>
+        <v>95.67751884460449</v>
       </c>
     </row>
     <row r="415" spans="1:4">
@@ -6523,10 +6523,10 @@
         <v>410</v>
       </c>
       <c r="C416">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D416">
-        <v>99.99914169311523</v>
+        <v>99.78752136230469</v>
       </c>
     </row>
     <row r="417" spans="1:4">
@@ -6537,7 +6537,7 @@
         <v>2</v>
       </c>
       <c r="D417">
-        <v>99.99995231628418</v>
+        <v>97.18581438064575</v>
       </c>
     </row>
     <row r="418" spans="1:4">
@@ -6548,7 +6548,7 @@
         <v>2</v>
       </c>
       <c r="D418">
-        <v>100</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="419" spans="1:4">
@@ -6570,7 +6570,7 @@
         <v>2</v>
       </c>
       <c r="D420">
-        <v>99.99998807907104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="421" spans="1:4">
@@ -6581,7 +6581,7 @@
         <v>2</v>
       </c>
       <c r="D421">
-        <v>99.99995231628418</v>
+        <v>100</v>
       </c>
     </row>
     <row r="422" spans="1:4">
@@ -6592,7 +6592,7 @@
         <v>2</v>
       </c>
       <c r="D422">
-        <v>99.99953508377075</v>
+        <v>100</v>
       </c>
     </row>
     <row r="423" spans="1:4">
@@ -6614,7 +6614,7 @@
         <v>2</v>
       </c>
       <c r="D424">
-        <v>99.99990463256836</v>
+        <v>99.99997615814209</v>
       </c>
     </row>
     <row r="425" spans="1:4">
@@ -6636,7 +6636,7 @@
         <v>2</v>
       </c>
       <c r="D426">
-        <v>99.99961853027344</v>
+        <v>99.99750852584839</v>
       </c>
     </row>
     <row r="427" spans="1:4">
@@ -6647,7 +6647,7 @@
         <v>2</v>
       </c>
       <c r="D427">
-        <v>99.99986886978149</v>
+        <v>99.99964237213135</v>
       </c>
     </row>
     <row r="428" spans="1:4">
@@ -6658,7 +6658,7 @@
         <v>1</v>
       </c>
       <c r="D428">
-        <v>99.99998807907104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="429" spans="1:4">
@@ -6669,7 +6669,7 @@
         <v>1</v>
       </c>
       <c r="D429">
-        <v>100</v>
+        <v>99.99997615814209</v>
       </c>
     </row>
     <row r="430" spans="1:4">
@@ -6691,7 +6691,7 @@
         <v>2</v>
       </c>
       <c r="D431">
-        <v>100</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="432" spans="1:4">
@@ -6713,7 +6713,7 @@
         <v>1</v>
       </c>
       <c r="D433">
-        <v>99.99998807907104</v>
+        <v>99.99984502792358</v>
       </c>
     </row>
     <row r="434" spans="1:4">
@@ -6746,7 +6746,7 @@
         <v>2</v>
       </c>
       <c r="D436">
-        <v>100</v>
+        <v>99.99991655349731</v>
       </c>
     </row>
     <row r="437" spans="1:4">
@@ -6757,7 +6757,7 @@
         <v>2</v>
       </c>
       <c r="D437">
-        <v>99.9997615814209</v>
+        <v>100</v>
       </c>
     </row>
     <row r="438" spans="1:4">
@@ -6768,7 +6768,7 @@
         <v>2</v>
       </c>
       <c r="D438">
-        <v>99.99868869781494</v>
+        <v>100</v>
       </c>
     </row>
     <row r="439" spans="1:4">
@@ -6801,7 +6801,7 @@
         <v>2</v>
       </c>
       <c r="D441">
-        <v>99.57855343818665</v>
+        <v>99.98860359191895</v>
       </c>
     </row>
     <row r="442" spans="1:4">
@@ -6812,7 +6812,7 @@
         <v>2</v>
       </c>
       <c r="D442">
-        <v>99.99998807907104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="443" spans="1:4">
@@ -6845,7 +6845,7 @@
         <v>2</v>
       </c>
       <c r="D445">
-        <v>100</v>
+        <v>99.9995231628418</v>
       </c>
     </row>
     <row r="446" spans="1:4">
@@ -6856,7 +6856,7 @@
         <v>2</v>
       </c>
       <c r="D446">
-        <v>99.99853372573853</v>
+        <v>99.96794462203979</v>
       </c>
     </row>
     <row r="447" spans="1:4">
@@ -6867,7 +6867,7 @@
         <v>2</v>
       </c>
       <c r="D447">
-        <v>100</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="448" spans="1:4">
@@ -6889,7 +6889,7 @@
         <v>2</v>
       </c>
       <c r="D449">
-        <v>99.99781847000122</v>
+        <v>99.99985694885254</v>
       </c>
     </row>
     <row r="450" spans="1:4">
@@ -6911,7 +6911,7 @@
         <v>2</v>
       </c>
       <c r="D451">
-        <v>99.99994039535522</v>
+        <v>99.99990463256836</v>
       </c>
     </row>
     <row r="452" spans="1:4">
@@ -6944,7 +6944,7 @@
         <v>2</v>
       </c>
       <c r="D454">
-        <v>99.99898672103882</v>
+        <v>99.99960660934448</v>
       </c>
     </row>
     <row r="455" spans="1:4">
@@ -6977,7 +6977,7 @@
         <v>2</v>
       </c>
       <c r="D457">
-        <v>99.99997615814209</v>
+        <v>99.9750554561615</v>
       </c>
     </row>
     <row r="458" spans="1:4">
@@ -7021,7 +7021,7 @@
         <v>2</v>
       </c>
       <c r="D461">
-        <v>99.99996423721313</v>
+        <v>99.99988079071045</v>
       </c>
     </row>
     <row r="462" spans="1:4">
@@ -7032,7 +7032,7 @@
         <v>2</v>
       </c>
       <c r="D462">
-        <v>100</v>
+        <v>99.99806880950928</v>
       </c>
     </row>
     <row r="463" spans="1:4">
@@ -7043,7 +7043,7 @@
         <v>2</v>
       </c>
       <c r="D463">
-        <v>99.99996423721313</v>
+        <v>99.99988079071045</v>
       </c>
     </row>
     <row r="464" spans="1:4">
@@ -7054,7 +7054,7 @@
         <v>2</v>
       </c>
       <c r="D464">
-        <v>99.99997615814209</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="465" spans="1:4">
@@ -7065,7 +7065,7 @@
         <v>2</v>
       </c>
       <c r="D465">
-        <v>99.99667406082153</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="466" spans="1:4">
@@ -7076,7 +7076,7 @@
         <v>2</v>
       </c>
       <c r="D466">
-        <v>99.99998807907104</v>
+        <v>99.99991655349731</v>
       </c>
     </row>
     <row r="467" spans="1:4">
@@ -7109,7 +7109,7 @@
         <v>2</v>
       </c>
       <c r="D469">
-        <v>99.99998807907104</v>
+        <v>99.99969005584717</v>
       </c>
     </row>
     <row r="470" spans="1:4">
@@ -7120,7 +7120,7 @@
         <v>1</v>
       </c>
       <c r="D470">
-        <v>99.99974966049194</v>
+        <v>99.99970197677612</v>
       </c>
     </row>
     <row r="471" spans="1:4">
@@ -7131,7 +7131,7 @@
         <v>1</v>
       </c>
       <c r="D471">
-        <v>99.99998807907104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="472" spans="1:4">
@@ -7142,7 +7142,7 @@
         <v>2</v>
       </c>
       <c r="D472">
-        <v>99.99998807907104</v>
+        <v>99.99997615814209</v>
       </c>
     </row>
     <row r="473" spans="1:4">
@@ -7153,7 +7153,7 @@
         <v>1</v>
       </c>
       <c r="D473">
-        <v>100</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="474" spans="1:4">
@@ -7164,7 +7164,7 @@
         <v>2</v>
       </c>
       <c r="D474">
-        <v>99.99992847442627</v>
+        <v>99.99737739562988</v>
       </c>
     </row>
     <row r="475" spans="1:4">
@@ -7208,7 +7208,7 @@
         <v>2</v>
       </c>
       <c r="D478">
-        <v>99.99998807907104</v>
+        <v>99.99964237213135</v>
       </c>
     </row>
     <row r="479" spans="1:4">
@@ -7285,7 +7285,7 @@
         <v>2</v>
       </c>
       <c r="D485">
-        <v>99.99998807907104</v>
+        <v>99.99997615814209</v>
       </c>
     </row>
     <row r="486" spans="1:4">
@@ -7296,7 +7296,7 @@
         <v>2</v>
       </c>
       <c r="D486">
-        <v>99.99998807907104</v>
+        <v>99.9998927116394</v>
       </c>
     </row>
     <row r="487" spans="1:4">
@@ -7307,7 +7307,7 @@
         <v>2</v>
       </c>
       <c r="D487">
-        <v>100</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="488" spans="1:4">
@@ -7318,7 +7318,7 @@
         <v>2</v>
       </c>
       <c r="D488">
-        <v>99.99994039535522</v>
+        <v>99.99986886978149</v>
       </c>
     </row>
     <row r="489" spans="1:4">
@@ -7329,7 +7329,7 @@
         <v>1</v>
       </c>
       <c r="D489">
-        <v>99.99995231628418</v>
+        <v>74.62078332901001</v>
       </c>
     </row>
     <row r="490" spans="1:4">
@@ -7337,10 +7337,10 @@
         <v>482</v>
       </c>
       <c r="C490">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D490">
-        <v>99.99099969863892</v>
+        <v>75.03392696380615</v>
       </c>
     </row>
     <row r="491" spans="1:4">
@@ -7351,7 +7351,7 @@
         <v>1</v>
       </c>
       <c r="D491">
-        <v>99.99954700469971</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="492" spans="1:4">
@@ -7373,7 +7373,7 @@
         <v>2</v>
       </c>
       <c r="D493">
-        <v>99.99995231628418</v>
+        <v>96.26237154006958</v>
       </c>
     </row>
     <row r="494" spans="1:4">
@@ -7384,7 +7384,7 @@
         <v>2</v>
       </c>
       <c r="D494">
-        <v>99.99710321426392</v>
+        <v>99.99986886978149</v>
       </c>
     </row>
     <row r="495" spans="1:4">
@@ -7406,7 +7406,7 @@
         <v>2</v>
       </c>
       <c r="D496">
-        <v>99.99992847442627</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="497" spans="1:4">
@@ -7417,7 +7417,7 @@
         <v>2</v>
       </c>
       <c r="D497">
-        <v>99.99964237213135</v>
+        <v>65.51699638366699</v>
       </c>
     </row>
     <row r="498" spans="1:4">
@@ -7428,7 +7428,7 @@
         <v>2</v>
       </c>
       <c r="D498">
-        <v>99.99977350234985</v>
+        <v>99.974125623703</v>
       </c>
     </row>
     <row r="499" spans="1:4">
@@ -7439,7 +7439,7 @@
         <v>2</v>
       </c>
       <c r="D499">
-        <v>99.9997615814209</v>
+        <v>99.99890327453613</v>
       </c>
     </row>
     <row r="500" spans="1:4">
@@ -7461,7 +7461,7 @@
         <v>2</v>
       </c>
       <c r="D501">
-        <v>100</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="502" spans="1:4">
@@ -7472,7 +7472,7 @@
         <v>2</v>
       </c>
       <c r="D502">
-        <v>99.99998807907104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="503" spans="1:4">
@@ -7483,7 +7483,7 @@
         <v>2</v>
       </c>
       <c r="D503">
-        <v>99.99960660934448</v>
+        <v>99.99731779098511</v>
       </c>
     </row>
     <row r="504" spans="1:4">
@@ -7494,7 +7494,7 @@
         <v>2</v>
       </c>
       <c r="D504">
-        <v>99.99994039535522</v>
+        <v>99.99997615814209</v>
       </c>
     </row>
     <row r="505" spans="1:4">
@@ -7505,7 +7505,7 @@
         <v>2</v>
       </c>
       <c r="D505">
-        <v>99.99998807907104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="506" spans="1:4">
@@ -7516,7 +7516,7 @@
         <v>2</v>
       </c>
       <c r="D506">
-        <v>99.99998807907104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="507" spans="1:4">
@@ -7527,7 +7527,7 @@
         <v>2</v>
       </c>
       <c r="D507">
-        <v>89.55191373825073</v>
+        <v>100</v>
       </c>
     </row>
     <row r="508" spans="1:4">
@@ -7571,7 +7571,7 @@
         <v>2</v>
       </c>
       <c r="D511">
-        <v>99.99997615814209</v>
+        <v>100</v>
       </c>
     </row>
     <row r="512" spans="1:4">
@@ -7582,7 +7582,7 @@
         <v>2</v>
       </c>
       <c r="D512">
-        <v>99.99998807907104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="513" spans="1:4">
@@ -7659,7 +7659,7 @@
         <v>2</v>
       </c>
       <c r="D519">
-        <v>99.99997615814209</v>
+        <v>99.99970197677612</v>
       </c>
     </row>
     <row r="520" spans="1:4">
@@ -7670,7 +7670,7 @@
         <v>1</v>
       </c>
       <c r="D520">
-        <v>98.01988005638123</v>
+        <v>70.11395692825317</v>
       </c>
     </row>
     <row r="521" spans="1:4">
@@ -7692,7 +7692,7 @@
         <v>2</v>
       </c>
       <c r="D522">
-        <v>99.98095631599426</v>
+        <v>100</v>
       </c>
     </row>
     <row r="523" spans="1:4">
@@ -7725,7 +7725,7 @@
         <v>1</v>
       </c>
       <c r="D525">
-        <v>99.99995231628418</v>
+        <v>99.99997615814209</v>
       </c>
     </row>
     <row r="526" spans="1:4">
@@ -7736,7 +7736,7 @@
         <v>1</v>
       </c>
       <c r="D526">
-        <v>99.99997615814209</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="527" spans="1:4">
@@ -7747,7 +7747,7 @@
         <v>1</v>
       </c>
       <c r="D527">
-        <v>100</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="528" spans="1:4">
@@ -7758,7 +7758,7 @@
         <v>1</v>
       </c>
       <c r="D528">
-        <v>100</v>
+        <v>99.99997615814209</v>
       </c>
     </row>
     <row r="529" spans="1:4">
@@ -7769,7 +7769,7 @@
         <v>2</v>
       </c>
       <c r="D529">
-        <v>99.98753070831299</v>
+        <v>99.99988079071045</v>
       </c>
     </row>
     <row r="530" spans="1:4">
@@ -7780,7 +7780,7 @@
         <v>2</v>
       </c>
       <c r="D530">
-        <v>99.9998927116394</v>
+        <v>99.99996423721313</v>
       </c>
     </row>
     <row r="531" spans="1:4">
@@ -7846,7 +7846,7 @@
         <v>2</v>
       </c>
       <c r="D536">
-        <v>99.6519923210144</v>
+        <v>100</v>
       </c>
     </row>
     <row r="537" spans="1:4">
@@ -7912,7 +7912,7 @@
         <v>1</v>
       </c>
       <c r="D542">
-        <v>99.99998807907104</v>
+        <v>99.99970197677612</v>
       </c>
     </row>
     <row r="543" spans="1:4">
@@ -7923,7 +7923,7 @@
         <v>1</v>
       </c>
       <c r="D543">
-        <v>100</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>